<commit_message>
Updated BOM for rev 1.2
</commit_message>
<xml_diff>
--- a/LVC_rev1/LVC_rev1_BOM.xlsx
+++ b/LVC_rev1/LVC_rev1_BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke\Documents\SSL\BPP\LVC\Eagle Files (Version Controlled)\LVC_rev1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke\Documents\SSL\Lipo Protection\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="90">
   <si>
     <t>Item #</t>
   </si>
@@ -278,7 +278,22 @@
     <t>R5, 6, 7, 11, 12, 13</t>
   </si>
   <si>
-    <t>UMD BPP Low Voltage Cutoff Rev 1.1 BOM</t>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>Murata</t>
+  </si>
+  <si>
+    <t>GRM188R71E104KA01D</t>
+  </si>
+  <si>
+    <t>0.10µF ±10% 25V X7R Ceramic Capacitor</t>
+  </si>
+  <si>
+    <t>490-1524-1-ND</t>
+  </si>
+  <si>
+    <t>UMD BPP Low Voltage Cutoff Rev 1.2 BOM</t>
   </si>
 </sst>
 </file>
@@ -685,10 +700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -704,7 +719,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -831,79 +846,83 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G5" s="6"/>
+        <v>86</v>
+      </c>
+      <c r="F5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="H5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>21</v>
+      <c r="I5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" t="s">
+        <v>88</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <f t="shared" ref="A6:A23" si="0">A5+1</f>
+        <f>A5+1</f>
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="C6" s="1">
-        <v>3</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="F6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>22</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="G6" s="6"/>
       <c r="H6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <f>A6+1</f>
+        <f t="shared" ref="A7:A24" si="0">A6+1</f>
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C7" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>73</v>
+        <v>23</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>22</v>
@@ -915,7 +934,7 @@
         <v>15</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -926,15 +945,15 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="C8" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>22</v>
@@ -946,7 +965,7 @@
         <v>15</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -957,15 +976,15 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C9" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>22</v>
@@ -977,7 +996,7 @@
         <v>15</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -988,22 +1007,18 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="C10" s="1">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>45</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>14</v>
@@ -1012,33 +1027,33 @@
         <v>15</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <f t="shared" si="0"/>
+        <f>A10+1</f>
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>14</v>
@@ -1047,33 +1062,33 @@
         <v>15</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <f>A11+1</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>14</v>
@@ -1081,8 +1096,8 @@
       <c r="I12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J12" t="s">
-        <v>77</v>
+      <c r="J12" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -1093,22 +1108,22 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>64</v>
+        <v>17</v>
       </c>
       <c r="C13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>14</v>
@@ -1116,8 +1131,8 @@
       <c r="I13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>48</v>
+      <c r="J13" t="s">
+        <v>77</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -1128,22 +1143,22 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="C14" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>14</v>
@@ -1151,8 +1166,8 @@
       <c r="I14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J14" t="s">
-        <v>61</v>
+      <c r="J14" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -1163,50 +1178,52 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="C15" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="1"/>
+        <v>68</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="F15" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" s="6"/>
+        <v>65</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="H15" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>55</v>
+        <v>15</v>
+      </c>
+      <c r="J15" t="s">
+        <v>61</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <f t="shared" si="0"/>
+        <f>A15+1</f>
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="C16" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E16" t="s">
-        <v>53</v>
-      </c>
+      <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="1" t="s">
@@ -1216,7 +1233,7 @@
         <v>19</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1227,19 +1244,29 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+        <v>80</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" t="s">
+        <v>53</v>
+      </c>
       <c r="F17" s="1" t="s">
-        <v>79</v>
+        <v>30</v>
       </c>
       <c r="G17" s="6"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+      <c r="H17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="J17" s="1" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -1249,14 +1276,21 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="G18" s="6"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
+      <c r="J18" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
@@ -1273,7 +1307,6 @@
       <c r="G19" s="6"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
     </row>
@@ -1345,6 +1378,23 @@
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
     </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:L1"/>

</xml_diff>